<commit_message>
Varios fixes realizados y mensajes de usuario
</commit_message>
<xml_diff>
--- a/templates/template_atencion_periodico.xlsx
+++ b/templates/template_atencion_periodico.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Atenciones" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Nombre</t>
   </si>
@@ -75,16 +75,13 @@
     <t>Semana Mes</t>
   </si>
   <si>
-    <t>Trimestre</t>
-  </si>
-  <si>
-    <t>Semestre</t>
+    <t>Periodo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -298,7 +295,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -333,7 +330,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -510,7 +507,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -518,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T8"/>
+  <dimension ref="A1:S8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,30 +532,30 @@
     <col min="7" max="7" width="25.42578125" style="1" customWidth="1"/>
     <col min="8" max="8" width="12" style="1" customWidth="1"/>
     <col min="9" max="10" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="13.85546875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="22.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="79.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.28515625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.7109375" style="1" customWidth="1"/>
-    <col min="17" max="17" width="14.5703125" style="1" customWidth="1"/>
-    <col min="18" max="18" width="18.42578125" style="1" customWidth="1"/>
-    <col min="19" max="19" width="59.140625" style="1" customWidth="1"/>
-    <col min="20" max="20" width="59.42578125" style="1" customWidth="1"/>
-    <col min="21" max="16384" width="9.140625" style="1"/>
+    <col min="11" max="11" width="13.85546875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="22.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="79.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.28515625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="14.5703125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="18.42578125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="59.140625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="59.42578125" style="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:20" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:19" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="6" t="s">
         <v>15</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="5" t="s">
         <v>0</v>
@@ -591,34 +588,31 @@
         <v>18</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="O5" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="P5" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="Q5" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="R5" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="S5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="T5" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C8" s="7"/>
     </row>
   </sheetData>

</xml_diff>